<commit_message>
add mean to results.xlsx
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan Su\Documents\GitHub\FinetuneLLM-NLP-Quiz\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8623CB40-A1F3-4180-AD31-78A746BBAB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEBF55C-9A18-4188-AF3A-FA386BA5A179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{18726F21-B83D-40FF-84A4-04DF132C406D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="925">
   <si>
     <t>case_id</t>
   </si>
@@ -2805,6 +2805,9 @@
   </si>
   <si>
     <t>atherosclerosis, thyroid nodule, liver cirrhosis, splenic lesion</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
 </sst>
 </file>
@@ -3306,7 +3309,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3316,9 +3319,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3695,10 +3695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F06E16-AE66-4B2E-A391-8EE15FF228E5}">
-  <dimension ref="A1:K245"/>
+  <dimension ref="A1:K246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C228" workbookViewId="0">
-      <selection activeCell="K244" sqref="K244"/>
+    <sheetView tabSelected="1" topLeftCell="C218" workbookViewId="0">
+      <selection activeCell="J248" sqref="J248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11549,10 +11549,39 @@
       </c>
     </row>
     <row r="245" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E245" s="6"/>
-      <c r="F245" s="6"/>
+      <c r="E245" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="F245" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="I245" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="J245" s="5" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="246" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E246" s="4">
+        <f>AVERAGE(E2:E237)</f>
+        <v>0.74288041415301853</v>
+      </c>
+      <c r="F246" s="4">
+        <f>AVERAGE(F2:F237)</f>
+        <v>0.74998102077809881</v>
+      </c>
+      <c r="I246" s="4">
+        <f>AVERAGE(I2:I237)</f>
+        <v>0.75036623501613464</v>
+      </c>
+      <c r="J246" s="4">
+        <f>AVERAGE(J2:J237)</f>
+        <v>0.76671821424095643</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix formatting in results.xlsx
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan Su\Documents\GitHub\FinetuneLLM-NLP-Quiz\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1D9A81-E96F-4307-BEFE-82542B87BB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8647DEDC-15EA-46C0-A6B8-75B08B41D3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{18726F21-B83D-40FF-84A4-04DF132C406D}"/>
   </bookViews>
@@ -3640,7 +3640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F06E16-AE66-4B2E-A391-8EE15FF228E5}">
   <dimension ref="A1:K243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
       <selection activeCell="J245" sqref="J245"/>
     </sheetView>
   </sheetViews>
@@ -3652,8 +3652,8 @@
     <col min="5" max="5" width="23.69140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="23.53515625" style="4" customWidth="1"/>
     <col min="7" max="8" width="23.69140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="24.53515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="24.765625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="23.84375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="23.921875" style="4" customWidth="1"/>
     <col min="11" max="11" width="23.84375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3714,10 +3714,10 @@
       <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>0.99999998013178504</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>0.99999998013178504</v>
       </c>
       <c r="K2" s="1"/>
@@ -3747,10 +3747,10 @@
       <c r="H3" s="3" t="s">
         <v>779</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>0.49964179098606099</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="4">
         <v>0.44117043912410697</v>
       </c>
       <c r="K3" s="1"/>
@@ -3780,10 +3780,10 @@
       <c r="H4" s="3" t="s">
         <v>780</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>0.851061731576919</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>0.86674258112907399</v>
       </c>
       <c r="K4" s="1"/>
@@ -3813,10 +3813,10 @@
       <c r="H5" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>0.98660504817962602</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="4">
         <v>1</v>
       </c>
       <c r="K5" s="1"/>
@@ -3846,10 +3846,10 @@
       <c r="H6" s="3" t="s">
         <v>781</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>0.85880175232887201</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="4">
         <v>0.89582175016403198</v>
       </c>
       <c r="K6" s="1"/>
@@ -3879,10 +3879,10 @@
       <c r="H7" s="3" t="s">
         <v>782</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <v>0.96882569789886397</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="4">
         <v>0.82719361782073897</v>
       </c>
       <c r="K7" s="1"/>
@@ -3912,10 +3912,10 @@
       <c r="H8" s="3" t="s">
         <v>783</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>0.87594095865885402</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <v>0.65049600973725297</v>
       </c>
       <c r="K8" s="1"/>
@@ -3945,10 +3945,10 @@
       <c r="H9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
         <v>1</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="4">
         <v>1</v>
       </c>
       <c r="K9" s="1"/>
@@ -3978,10 +3978,10 @@
       <c r="H10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="4">
         <v>0.81577607989311196</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="4">
         <v>0.79156929254531805</v>
       </c>
       <c r="K10" s="1"/>
@@ -4011,10 +4011,10 @@
       <c r="H11" s="3" t="s">
         <v>784</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="4">
         <v>0.89578464627265897</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="4">
         <v>0.76574503630399704</v>
       </c>
       <c r="K11" s="1"/>
@@ -4044,10 +4044,10 @@
       <c r="H12" s="3" t="s">
         <v>785</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="4">
         <v>0.90017408132553101</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="4">
         <v>0.65798303484916598</v>
       </c>
       <c r="K12" s="1"/>
@@ -4077,10 +4077,10 @@
       <c r="H13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="4">
         <v>0.96863827109336798</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="4">
         <v>0.83233422040939298</v>
       </c>
       <c r="K13" s="1"/>
@@ -4110,10 +4110,10 @@
       <c r="H14" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="4">
         <v>0.81577607989311196</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="4">
         <v>0.74131402373313904</v>
       </c>
       <c r="K14" s="1"/>
@@ -4143,10 +4143,10 @@
       <c r="H15" s="3" t="s">
         <v>787</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="4">
         <v>0.80579022566477398</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="4">
         <v>0.75923298299312503</v>
       </c>
       <c r="K15" s="1"/>
@@ -4176,10 +4176,10 @@
       <c r="H16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="4">
         <v>1</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="4">
         <v>1</v>
       </c>
       <c r="K16" s="1"/>
@@ -4209,10 +4209,10 @@
       <c r="H17" s="3" t="s">
         <v>788</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="4">
         <v>0.55352979898452703</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="4">
         <v>0.55352979898452703</v>
       </c>
       <c r="K17" s="1"/>
@@ -4242,10 +4242,10 @@
       <c r="H18" s="3" t="s">
         <v>789</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="4">
         <v>0.65613591670989901</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="4">
         <v>0.75837792952855398</v>
       </c>
       <c r="K18" s="1"/>
@@ -4275,10 +4275,10 @@
       <c r="H19" s="3" t="s">
         <v>790</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="4">
         <v>0.60541138052940302</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <v>0.78759735822677601</v>
       </c>
       <c r="K19" s="1"/>
@@ -4308,10 +4308,10 @@
       <c r="H20" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="4">
         <v>0.80574935674667303</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="4">
         <v>0.79542900621891</v>
       </c>
       <c r="K20" s="1"/>
@@ -4341,10 +4341,10 @@
       <c r="H21" s="3" t="s">
         <v>792</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="4">
         <v>1.0000000149011601</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="4">
         <v>0.95502176880836398</v>
       </c>
       <c r="K21" s="1"/>
@@ -4374,10 +4374,10 @@
       <c r="H22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="4">
         <v>0.83083805441856295</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="4">
         <v>0.88605058193206698</v>
       </c>
       <c r="K22" s="1"/>
@@ -4407,10 +4407,10 @@
       <c r="H23" s="3" t="s">
         <v>793</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="4">
         <v>0.72857535630464498</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="4">
         <v>0.64331524570782905</v>
       </c>
       <c r="K23" s="1"/>
@@ -4440,10 +4440,10 @@
       <c r="H24" s="3" t="s">
         <v>794</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="4">
         <v>0.95287695527076699</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="4">
         <v>0.99778437614440896</v>
       </c>
       <c r="K24" s="1"/>
@@ -4473,10 +4473,10 @@
       <c r="H25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="4">
         <v>0.64592093229293801</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="4">
         <v>0.47421866655349698</v>
       </c>
       <c r="K25" s="1"/>
@@ -4506,10 +4506,10 @@
       <c r="H26" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="4">
         <v>0.783744476735591</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="4">
         <v>0.88637749354044504</v>
       </c>
       <c r="K26" s="1"/>
@@ -4539,10 +4539,10 @@
       <c r="H27" s="3" t="s">
         <v>795</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="4">
         <v>0.52013291418552399</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="4">
         <v>0.630446597933769</v>
       </c>
       <c r="K27" s="1"/>
@@ -4572,10 +4572,10 @@
       <c r="H28" s="3" t="s">
         <v>796</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="4">
         <v>0.96495440602302496</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="4">
         <v>0.96863827109336798</v>
       </c>
       <c r="K28" s="1"/>
@@ -4605,10 +4605,10 @@
       <c r="H29" s="3" t="s">
         <v>797</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="4">
         <v>0.79445064067840498</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="4">
         <v>0.75268542766571001</v>
       </c>
       <c r="K29" s="1"/>
@@ -4638,10 +4638,10 @@
       <c r="H30" s="3" t="s">
         <v>798</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="4">
         <v>0.77486801147460904</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="4">
         <v>0.90199670195579496</v>
       </c>
       <c r="K30" s="1"/>
@@ -4671,10 +4671,10 @@
       <c r="H31" s="3" t="s">
         <v>799</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="4">
         <v>1</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="4">
         <v>1</v>
       </c>
       <c r="K31" s="1"/>
@@ -4704,10 +4704,10 @@
       <c r="H32" s="3" t="s">
         <v>800</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="4">
         <v>0.75936815142631497</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="4">
         <v>0.72229206065336804</v>
       </c>
       <c r="K32" s="1"/>
@@ -4737,10 +4737,10 @@
       <c r="H33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="4">
         <v>0.99999997019767695</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="4">
         <v>0.99999997019767695</v>
       </c>
       <c r="K33" s="1"/>
@@ -4770,10 +4770,10 @@
       <c r="H34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="4">
         <v>0.85558956861495905</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="4">
         <v>0.85558956861495905</v>
       </c>
       <c r="K34" s="1"/>
@@ -4803,10 +4803,10 @@
       <c r="H35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="4">
         <v>1</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="4">
         <v>1</v>
       </c>
       <c r="K35" s="1"/>
@@ -4836,10 +4836,10 @@
       <c r="H36" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="4">
         <v>0.999999940395355</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="4">
         <v>0.659132480621337</v>
       </c>
       <c r="K36" s="1"/>
@@ -4869,10 +4869,10 @@
       <c r="H37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="4">
         <v>0.74535532792409198</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="4">
         <v>0.99999997019767695</v>
       </c>
       <c r="K37" s="1"/>
@@ -4902,10 +4902,10 @@
       <c r="H38" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="4">
         <v>1</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="4">
         <v>1</v>
       </c>
       <c r="K38" s="1"/>
@@ -4935,10 +4935,10 @@
       <c r="H39" s="3" t="s">
         <v>801</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="4">
         <v>0.65267425775527899</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="4">
         <v>0.802943795919418</v>
       </c>
       <c r="K39" s="1"/>
@@ -4968,10 +4968,10 @@
       <c r="H40" s="3" t="s">
         <v>802</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="4">
         <v>0.63155215978622403</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="4">
         <v>0.80082666873931796</v>
       </c>
       <c r="K40" s="1"/>
@@ -5001,10 +5001,10 @@
       <c r="H41" s="3" t="s">
         <v>803</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="4">
         <v>0.85236735343933101</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="4">
         <v>0.82556803226470898</v>
       </c>
       <c r="K41" s="1"/>
@@ -5034,10 +5034,10 @@
       <c r="H42" s="3" t="s">
         <v>804</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="4">
         <v>0.82092060645421305</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="4">
         <v>0.79658212264378803</v>
       </c>
       <c r="K42" s="1"/>
@@ -5067,10 +5067,10 @@
       <c r="H43" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="4">
         <v>0.88996568322181702</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="4">
         <v>0.605217784643173</v>
       </c>
       <c r="K43" s="1"/>
@@ -5100,10 +5100,10 @@
       <c r="H44" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="4">
         <v>0.78430225451787305</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="4">
         <v>0.78064054250717096</v>
       </c>
       <c r="K44" s="1"/>
@@ -5133,10 +5133,10 @@
       <c r="H45" s="3" t="s">
         <v>805</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="4">
         <v>0.92246052622795105</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="4">
         <v>0.52967828512191695</v>
       </c>
       <c r="K45" s="1"/>
@@ -5160,10 +5160,10 @@
       <c r="G46" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="4">
         <v>0.82594674825668302</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="4">
         <v>0.16610771417617701</v>
       </c>
       <c r="K46" s="1"/>
@@ -5193,10 +5193,10 @@
       <c r="H47" s="3" t="s">
         <v>806</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="4">
         <v>0.63860351840655005</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="4">
         <v>0.66927124063173904</v>
       </c>
       <c r="K47" s="1"/>
@@ -5226,10 +5226,10 @@
       <c r="H48" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="4">
         <v>0.67762017250061002</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="4">
         <v>0.67762017250061002</v>
       </c>
       <c r="K48" s="1"/>
@@ -5259,10 +5259,10 @@
       <c r="H49" s="3" t="s">
         <v>807</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="4">
         <v>0.99999996026356996</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="4">
         <v>0.87080601851145401</v>
       </c>
       <c r="K49" s="1"/>
@@ -5280,10 +5280,10 @@
       <c r="F50" s="4">
         <v>0.22638063132762901</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="4">
         <v>0.22638063132762901</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="4">
         <v>0.22638063132762901</v>
       </c>
       <c r="K50" s="1"/>
@@ -5313,10 +5313,10 @@
       <c r="H51" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="4">
         <v>1.00000001986821</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="4">
         <v>0.96863827109336798</v>
       </c>
       <c r="K51" s="1"/>
@@ -5346,10 +5346,10 @@
       <c r="H52" s="3" t="s">
         <v>808</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="4">
         <v>0.70650571584701505</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="4">
         <v>0.659839928150177</v>
       </c>
       <c r="K52" s="1"/>
@@ -5379,10 +5379,10 @@
       <c r="H53" s="3" t="s">
         <v>809</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="4">
         <v>0.83401294549306204</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="4">
         <v>1</v>
       </c>
       <c r="K53" s="1"/>
@@ -5412,10 +5412,10 @@
       <c r="H54" s="3" t="s">
         <v>810</v>
       </c>
-      <c r="I54">
+      <c r="I54" s="4">
         <v>0.85708896319071404</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="4">
         <v>0.771619458993276</v>
       </c>
       <c r="K54" s="1"/>
@@ -5445,10 +5445,10 @@
       <c r="H55" s="3" t="s">
         <v>811</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="4">
         <v>0.75020027160644498</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="4">
         <v>0.533095349868138</v>
       </c>
       <c r="K55" s="1"/>
@@ -5478,10 +5478,10 @@
       <c r="H56" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="4">
         <v>0.83338860670725501</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="4">
         <v>0.88965448737144404</v>
       </c>
       <c r="K56" s="1"/>
@@ -5511,10 +5511,10 @@
       <c r="H57" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="4">
         <v>0.59973746538162198</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="4">
         <v>0.53492907683054602</v>
       </c>
       <c r="K57" s="1"/>
@@ -5544,10 +5544,10 @@
       <c r="H58" s="3" t="s">
         <v>812</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="4">
         <v>0.73710945248603799</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="4">
         <v>0.81742382049560502</v>
       </c>
       <c r="K58" s="1"/>
@@ -5577,10 +5577,10 @@
       <c r="H59" s="3" t="s">
         <v>813</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="4">
         <v>0.690788221359252</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="4">
         <v>0.68798810541629796</v>
       </c>
       <c r="K59" s="1"/>
@@ -5610,10 +5610,10 @@
       <c r="H60" s="3" t="s">
         <v>814</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="4">
         <v>0.75035083293914795</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="4">
         <v>0.29144170880317599</v>
       </c>
       <c r="K60" s="1"/>
@@ -5643,10 +5643,10 @@
       <c r="H61" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="4">
         <v>0.63155215978622403</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="4">
         <v>0.63155215978622403</v>
       </c>
       <c r="K61" s="1"/>
@@ -5676,10 +5676,10 @@
       <c r="H62" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="4">
         <v>1.00000023841857</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="4">
         <v>0.625701904296875</v>
       </c>
       <c r="K62" s="1"/>
@@ -5709,10 +5709,10 @@
       <c r="H63" s="3" t="s">
         <v>815</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="4">
         <v>0.56813042610883702</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="4">
         <v>0.82725313901901198</v>
       </c>
       <c r="K63" s="1"/>
@@ -5742,10 +5742,10 @@
       <c r="H64" s="3" t="s">
         <v>816</v>
       </c>
-      <c r="I64">
+      <c r="I64" s="4">
         <v>0.67351970076560896</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="4">
         <v>0.81012431780497196</v>
       </c>
       <c r="K64" s="1"/>
@@ -5775,10 +5775,10 @@
       <c r="H65" s="3" t="s">
         <v>817</v>
       </c>
-      <c r="I65">
+      <c r="I65" s="4">
         <v>0.92089039087295499</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="4">
         <v>0.86204278469085605</v>
       </c>
       <c r="K65" s="1"/>
@@ -5808,10 +5808,10 @@
       <c r="H66" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="I66">
+      <c r="I66" s="4">
         <v>0.63583363095919199</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="4">
         <v>0.59138959646224898</v>
       </c>
       <c r="K66" s="1"/>
@@ -5841,10 +5841,10 @@
       <c r="H67" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="I67">
+      <c r="I67" s="4">
         <v>0.227014601230621</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="4">
         <v>0.227014601230621</v>
       </c>
       <c r="K67" s="1"/>
@@ -5874,10 +5874,10 @@
       <c r="H68" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="4">
         <v>0.92246052622795105</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="4">
         <v>0.84368231892585699</v>
       </c>
       <c r="K68" s="1"/>
@@ -5907,10 +5907,10 @@
       <c r="H69" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="I69">
+      <c r="I69" s="4">
         <v>0.60642156004905701</v>
       </c>
-      <c r="J69">
+      <c r="J69" s="4">
         <v>0.26995798821250599</v>
       </c>
       <c r="K69" s="1"/>
@@ -5937,10 +5937,10 @@
       <c r="H70" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="I70">
+      <c r="I70" s="4">
         <v>0.48693448305129999</v>
       </c>
-      <c r="J70">
+      <c r="J70" s="4">
         <v>0.48693448305129999</v>
       </c>
       <c r="K70" s="1"/>
@@ -5970,10 +5970,10 @@
       <c r="H71" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="I71">
+      <c r="I71" s="4">
         <v>0.69036905467510201</v>
       </c>
-      <c r="J71">
+      <c r="J71" s="4">
         <v>0.86084529757499695</v>
       </c>
       <c r="K71" s="1"/>
@@ -6003,10 +6003,10 @@
       <c r="H72" s="3" t="s">
         <v>821</v>
       </c>
-      <c r="I72">
+      <c r="I72" s="4">
         <v>0.380455821752548</v>
       </c>
-      <c r="J72">
+      <c r="J72" s="4">
         <v>0.37276154756545998</v>
       </c>
       <c r="K72" s="1"/>
@@ -6036,10 +6036,10 @@
       <c r="H73" s="3" t="s">
         <v>822</v>
       </c>
-      <c r="I73">
+      <c r="I73" s="4">
         <v>0.78720887005329099</v>
       </c>
-      <c r="J73">
+      <c r="J73" s="4">
         <v>0.65314877033233598</v>
       </c>
       <c r="K73" s="1"/>
@@ -6069,10 +6069,10 @@
       <c r="H74" s="3" t="s">
         <v>823</v>
       </c>
-      <c r="I74">
+      <c r="I74" s="4">
         <v>0.81713497638702304</v>
       </c>
-      <c r="J74">
+      <c r="J74" s="4">
         <v>0.82271793484687805</v>
       </c>
       <c r="K74" s="1"/>
@@ -6102,10 +6102,10 @@
       <c r="H75" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I75">
+      <c r="I75" s="4">
         <v>0.41947683691978399</v>
       </c>
-      <c r="J75">
+      <c r="J75" s="4">
         <v>0.41947683691978399</v>
       </c>
       <c r="K75" s="1"/>
@@ -6135,10 +6135,10 @@
       <c r="H76" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="I76">
+      <c r="I76" s="4">
         <v>0.62211651355028097</v>
       </c>
-      <c r="J76">
+      <c r="J76" s="4">
         <v>0.70447383324305202</v>
       </c>
       <c r="K76" s="1"/>
@@ -6168,10 +6168,10 @@
       <c r="H77" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="I77">
+      <c r="I77" s="4">
         <v>0.91782541573047605</v>
       </c>
-      <c r="J77">
+      <c r="J77" s="4">
         <v>0.99852289756139101</v>
       </c>
       <c r="K77" s="1"/>
@@ -6201,10 +6201,10 @@
       <c r="H78" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I78">
+      <c r="I78" s="4">
         <v>0.89636671543121305</v>
       </c>
-      <c r="J78">
+      <c r="J78" s="4">
         <v>0.69907957315444902</v>
       </c>
       <c r="K78" s="1"/>
@@ -6234,10 +6234,10 @@
       <c r="H79" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="I79">
+      <c r="I79" s="4">
         <v>0.66195499897003096</v>
       </c>
-      <c r="J79">
+      <c r="J79" s="4">
         <v>0.99556875228881803</v>
       </c>
       <c r="K79" s="1"/>
@@ -6267,10 +6267,10 @@
       <c r="H80" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I80">
+      <c r="I80" s="4">
         <v>1</v>
       </c>
-      <c r="J80">
+      <c r="J80" s="4">
         <v>1</v>
       </c>
       <c r="K80" s="1"/>
@@ -6300,10 +6300,10 @@
       <c r="H81" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="I81">
+      <c r="I81" s="4">
         <v>0.74346736073493902</v>
       </c>
-      <c r="J81">
+      <c r="J81" s="4">
         <v>0.74346736073493902</v>
       </c>
       <c r="K81" s="1"/>
@@ -6333,10 +6333,10 @@
       <c r="H82" s="3" t="s">
         <v>826</v>
       </c>
-      <c r="I82">
+      <c r="I82" s="4">
         <v>0.83881008625030495</v>
       </c>
-      <c r="J82">
+      <c r="J82" s="4">
         <v>0.83881008625030495</v>
       </c>
       <c r="K82" s="1"/>
@@ -6366,10 +6366,10 @@
       <c r="H83" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="I83">
+      <c r="I83" s="4">
         <v>0.73854660987854004</v>
       </c>
-      <c r="J83">
+      <c r="J83" s="4">
         <v>0.83928896983464496</v>
       </c>
       <c r="K83" s="1"/>
@@ -6399,10 +6399,10 @@
       <c r="H84" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I84">
+      <c r="I84" s="4">
         <v>0.84234872460365295</v>
       </c>
-      <c r="J84">
+      <c r="J84" s="4">
         <v>0.74639800190925598</v>
       </c>
       <c r="K84" s="1"/>
@@ -6432,10 +6432,10 @@
       <c r="H85" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="I85">
+      <c r="I85" s="4">
         <v>0.787923137346903</v>
       </c>
-      <c r="J85">
+      <c r="J85" s="4">
         <v>0.79876006642977304</v>
       </c>
       <c r="K85" s="1"/>
@@ -6465,10 +6465,10 @@
       <c r="H86" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="I86">
+      <c r="I86" s="4">
         <v>0.90859135985374395</v>
       </c>
-      <c r="J86">
+      <c r="J86" s="4">
         <v>0.71328727900981903</v>
       </c>
       <c r="K86" s="1"/>
@@ -6498,10 +6498,10 @@
       <c r="H87" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="I87">
+      <c r="I87" s="4">
         <v>0.82409293949604001</v>
       </c>
-      <c r="J87">
+      <c r="J87" s="4">
         <v>0.72007629275321905</v>
       </c>
       <c r="K87" s="1"/>
@@ -6531,10 +6531,10 @@
       <c r="H88" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="I88">
+      <c r="I88" s="4">
         <v>0.83554640412330605</v>
       </c>
-      <c r="J88">
+      <c r="J88" s="4">
         <v>0.78441435098648005</v>
       </c>
       <c r="K88" s="1"/>
@@ -6564,10 +6564,10 @@
       <c r="H89" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="I89">
+      <c r="I89" s="4">
         <v>0.60031959414482094</v>
       </c>
-      <c r="J89">
+      <c r="J89" s="4">
         <v>0.66068530082702603</v>
       </c>
       <c r="K89" s="1"/>
@@ -6585,10 +6585,10 @@
       <c r="F90" s="4">
         <v>0.13911400735378199</v>
       </c>
-      <c r="I90">
+      <c r="I90" s="4">
         <v>0.13911400735378199</v>
       </c>
-      <c r="J90">
+      <c r="J90" s="4">
         <v>0.13911400735378199</v>
       </c>
       <c r="K90" s="1"/>
@@ -6618,10 +6618,10 @@
       <c r="H91" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I91">
+      <c r="I91" s="4">
         <v>0.88611471652984597</v>
       </c>
-      <c r="J91">
+      <c r="J91" s="4">
         <v>0.97909218072891202</v>
       </c>
       <c r="K91" s="1"/>
@@ -6651,10 +6651,10 @@
       <c r="H92" s="3" t="s">
         <v>832</v>
       </c>
-      <c r="I92">
+      <c r="I92" s="4">
         <v>0.84898251295089699</v>
       </c>
-      <c r="J92">
+      <c r="J92" s="4">
         <v>0.84462271928787203</v>
       </c>
       <c r="K92" s="1"/>
@@ -6684,10 +6684,10 @@
       <c r="H93" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="I93">
+      <c r="I93" s="4">
         <v>0.87080601851145401</v>
       </c>
-      <c r="J93">
+      <c r="J93" s="4">
         <v>0.96863827109336798</v>
       </c>
       <c r="K93" s="1"/>
@@ -6717,10 +6717,10 @@
       <c r="H94" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="I94">
+      <c r="I94" s="4">
         <v>0.71267257630824998</v>
       </c>
-      <c r="J94">
+      <c r="J94" s="4">
         <v>0.65144119660059596</v>
       </c>
       <c r="K94" s="1"/>
@@ -6750,10 +6750,10 @@
       <c r="H95" s="3" t="s">
         <v>834</v>
       </c>
-      <c r="I95">
+      <c r="I95" s="4">
         <v>0.67055912315845401</v>
       </c>
-      <c r="J95">
+      <c r="J95" s="4">
         <v>0.87323850393295199</v>
       </c>
       <c r="K95" s="1"/>
@@ -6783,10 +6783,10 @@
       <c r="H96" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I96">
+      <c r="I96" s="4">
         <v>0.93727654218673695</v>
       </c>
-      <c r="J96">
+      <c r="J96" s="4">
         <v>0.999999940395355</v>
       </c>
       <c r="K96" s="1"/>
@@ -6816,10 +6816,10 @@
       <c r="H97" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I97">
+      <c r="I97" s="4">
         <v>0.96863827109336798</v>
       </c>
-      <c r="J97">
+      <c r="J97" s="4">
         <v>1</v>
       </c>
       <c r="K97" s="1"/>
@@ -6849,10 +6849,10 @@
       <c r="H98" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="I98">
+      <c r="I98" s="4">
         <v>0.79672735929489102</v>
       </c>
-      <c r="J98">
+      <c r="J98" s="4">
         <v>0.84368228912353505</v>
       </c>
       <c r="K98" s="1"/>
@@ -6882,10 +6882,10 @@
       <c r="H99" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="I99">
+      <c r="I99" s="4">
         <v>0.86054079532623295</v>
       </c>
-      <c r="J99">
+      <c r="J99" s="4">
         <v>0.88045017421245497</v>
       </c>
       <c r="K99" s="1"/>
@@ -6915,10 +6915,10 @@
       <c r="H100" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="I100">
+      <c r="I100" s="4">
         <v>1</v>
       </c>
-      <c r="J100">
+      <c r="J100" s="4">
         <v>1</v>
       </c>
       <c r="K100" s="1"/>
@@ -6948,10 +6948,10 @@
       <c r="H101" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="I101">
+      <c r="I101" s="4">
         <v>0.85136374831199602</v>
       </c>
-      <c r="J101">
+      <c r="J101" s="4">
         <v>0.82956624031066895</v>
       </c>
       <c r="K101" s="1"/>
@@ -6981,10 +6981,10 @@
       <c r="H102" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="I102">
+      <c r="I102" s="4">
         <v>0.67762017250061002</v>
       </c>
-      <c r="J102">
+      <c r="J102" s="4">
         <v>0.83659446239471402</v>
       </c>
       <c r="K102" s="1"/>
@@ -7014,10 +7014,10 @@
       <c r="H103" s="3" t="s">
         <v>837</v>
       </c>
-      <c r="I103">
+      <c r="I103" s="4">
         <v>0.26645958423614502</v>
       </c>
-      <c r="J103">
+      <c r="J103" s="4">
         <v>0.27410018444061202</v>
       </c>
       <c r="K103" s="1"/>
@@ -7047,10 +7047,10 @@
       <c r="H104" s="3" t="s">
         <v>838</v>
       </c>
-      <c r="I104">
+      <c r="I104" s="4">
         <v>0.4989964812994</v>
       </c>
-      <c r="J104">
+      <c r="J104" s="4">
         <v>0.59527246654033605</v>
       </c>
       <c r="K104" s="1"/>
@@ -7080,10 +7080,10 @@
       <c r="H105" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="I105">
+      <c r="I105" s="4">
         <v>0.97867506742477395</v>
       </c>
-      <c r="J105">
+      <c r="J105" s="4">
         <v>0.87517541646957397</v>
       </c>
       <c r="K105" s="1"/>
@@ -7113,10 +7113,10 @@
       <c r="H106" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="I106">
+      <c r="I106" s="4">
         <v>0.81829434633255005</v>
       </c>
-      <c r="J106">
+      <c r="J106" s="4">
         <v>0.81829434633255005</v>
       </c>
       <c r="K106" s="1"/>
@@ -7146,10 +7146,10 @@
       <c r="H107" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="I107">
+      <c r="I107" s="4">
         <v>0.99167957901954595</v>
       </c>
-      <c r="J107">
+      <c r="J107" s="4">
         <v>0.83881008625030495</v>
       </c>
       <c r="K107" s="1"/>
@@ -7179,10 +7179,10 @@
       <c r="H108" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I108">
+      <c r="I108" s="4">
         <v>0.96863827109336798</v>
       </c>
-      <c r="J108">
+      <c r="J108" s="4">
         <v>0.999999940395355</v>
       </c>
       <c r="K108" s="1"/>
@@ -7212,10 +7212,10 @@
       <c r="H109" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="I109">
+      <c r="I109" s="4">
         <v>0.65598232547442104</v>
       </c>
-      <c r="J109">
+      <c r="J109" s="4">
         <v>0.62600362300872803</v>
       </c>
       <c r="K109" s="1"/>
@@ -7245,10 +7245,10 @@
       <c r="H110" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I110">
+      <c r="I110" s="4">
         <v>0.93727654218673695</v>
       </c>
-      <c r="J110">
+      <c r="J110" s="4">
         <v>0.999999940395355</v>
       </c>
       <c r="K110" s="1"/>
@@ -7278,10 +7278,10 @@
       <c r="H111" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="I111">
+      <c r="I111" s="4">
         <v>0.70210994283358197</v>
       </c>
-      <c r="J111">
+      <c r="J111" s="4">
         <v>0.82189408938090003</v>
       </c>
       <c r="K111" s="1"/>
@@ -7311,10 +7311,10 @@
       <c r="H112" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="I112">
+      <c r="I112" s="4">
         <v>0.75433379411697299</v>
       </c>
-      <c r="J112">
+      <c r="J112" s="4">
         <v>0.75433379411697299</v>
       </c>
       <c r="K112" s="1"/>
@@ -7344,10 +7344,10 @@
       <c r="H113" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="I113">
+      <c r="I113" s="4">
         <v>0.81391134858131398</v>
       </c>
-      <c r="J113">
+      <c r="J113" s="4">
         <v>0.81391134858131398</v>
       </c>
       <c r="K113" s="1"/>
@@ -7377,10 +7377,10 @@
       <c r="H114" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="I114">
+      <c r="I114" s="4">
         <v>0.79915148019790605</v>
       </c>
-      <c r="J114">
+      <c r="J114" s="4">
         <v>0.80948385596275296</v>
       </c>
       <c r="K114" s="1"/>
@@ -7410,10 +7410,10 @@
       <c r="H115" s="3" t="s">
         <v>843</v>
       </c>
-      <c r="I115">
+      <c r="I115" s="4">
         <v>0.96863827109336798</v>
       </c>
-      <c r="J115">
+      <c r="J115" s="4">
         <v>0.99999997019767695</v>
       </c>
       <c r="K115" s="1"/>
@@ -7443,10 +7443,10 @@
       <c r="H116" s="3" t="s">
         <v>844</v>
       </c>
-      <c r="I116">
+      <c r="I116" s="4">
         <v>0.720037107666333</v>
       </c>
-      <c r="J116">
+      <c r="J116" s="4">
         <v>0.75276003281275405</v>
       </c>
       <c r="K116" s="1"/>
@@ -7476,10 +7476,10 @@
       <c r="H117" s="3" t="s">
         <v>845</v>
       </c>
-      <c r="I117">
+      <c r="I117" s="4">
         <v>0.91478312015533403</v>
       </c>
-      <c r="J117">
+      <c r="J117" s="4">
         <v>0.92476989328861203</v>
       </c>
       <c r="K117" s="1"/>
@@ -7509,10 +7509,10 @@
       <c r="H118" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="I118">
+      <c r="I118" s="4">
         <v>0.47147598862647999</v>
       </c>
-      <c r="J118">
+      <c r="J118" s="4">
         <v>0.52000087499618497</v>
       </c>
       <c r="K118" s="1"/>
@@ -7542,10 +7542,10 @@
       <c r="H119" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="I119">
+      <c r="I119" s="4">
         <v>0.63155215978622403</v>
       </c>
-      <c r="J119">
+      <c r="J119" s="4">
         <v>0.61687356233596802</v>
       </c>
       <c r="K119" s="1"/>
@@ -7575,10 +7575,10 @@
       <c r="H120" s="3" t="s">
         <v>847</v>
       </c>
-      <c r="I120">
+      <c r="I120" s="4">
         <v>0.97909218072891202</v>
       </c>
-      <c r="J120">
+      <c r="J120" s="4">
         <v>0.90719419717788696</v>
       </c>
       <c r="K120" s="1"/>
@@ -7608,10 +7608,10 @@
       <c r="H121" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I121">
+      <c r="I121" s="4">
         <v>0.81178206205367998</v>
       </c>
-      <c r="J121">
+      <c r="J121" s="4">
         <v>0.999999940395355</v>
       </c>
       <c r="K121" s="1"/>
@@ -7641,10 +7641,10 @@
       <c r="H122" s="3" t="s">
         <v>848</v>
       </c>
-      <c r="I122">
+      <c r="I122" s="4">
         <v>0.81174094974994604</v>
       </c>
-      <c r="J122">
+      <c r="J122" s="4">
         <v>0.99999998509883803</v>
       </c>
       <c r="K122" s="1"/>
@@ -7674,10 +7674,10 @@
       <c r="H123" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="I123">
+      <c r="I123" s="4">
         <v>0.70527774095535201</v>
       </c>
-      <c r="J123">
+      <c r="J123" s="4">
         <v>0.712105512619018</v>
       </c>
       <c r="K123" s="1"/>
@@ -7707,10 +7707,10 @@
       <c r="H124" s="3" t="s">
         <v>849</v>
       </c>
-      <c r="I124">
+      <c r="I124" s="4">
         <v>0.62564671039581299</v>
       </c>
-      <c r="J124">
+      <c r="J124" s="4">
         <v>1</v>
       </c>
       <c r="K124" s="1"/>
@@ -7740,10 +7740,10 @@
       <c r="H125" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="I125">
+      <c r="I125" s="4">
         <v>0.83836883306503296</v>
       </c>
-      <c r="J125">
+      <c r="J125" s="4">
         <v>0.94921702146530096</v>
       </c>
       <c r="K125" s="1"/>
@@ -7773,10 +7773,10 @@
       <c r="H126" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I126">
+      <c r="I126" s="4">
         <v>0.93727654218673695</v>
       </c>
-      <c r="J126">
+      <c r="J126" s="4">
         <v>0.999999940395355</v>
       </c>
       <c r="K126" s="1"/>
@@ -7806,10 +7806,10 @@
       <c r="H127" s="3" t="s">
         <v>851</v>
       </c>
-      <c r="I127">
+      <c r="I127" s="4">
         <v>0.736723268032074</v>
       </c>
-      <c r="J127">
+      <c r="J127" s="4">
         <v>0.67795057098070699</v>
       </c>
       <c r="K127" s="1"/>
@@ -7839,10 +7839,10 @@
       <c r="H128" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="I128">
+      <c r="I128" s="4">
         <v>0.80394139885902405</v>
       </c>
-      <c r="J128">
+      <c r="J128" s="4">
         <v>0.99999997019767695</v>
       </c>
       <c r="K128" s="1"/>
@@ -7872,10 +7872,10 @@
       <c r="H129" s="3" t="s">
         <v>607</v>
       </c>
-      <c r="I129">
+      <c r="I129" s="4">
         <v>0.72827111184597004</v>
       </c>
-      <c r="J129">
+      <c r="J129" s="4">
         <v>0.66631846129894201</v>
       </c>
       <c r="K129" s="1"/>
@@ -7905,10 +7905,10 @@
       <c r="H130" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="I130">
+      <c r="I130" s="4">
         <v>0.83297753334045399</v>
       </c>
-      <c r="J130">
+      <c r="J130" s="4">
         <v>0.41970948378244999</v>
       </c>
       <c r="K130" s="1"/>
@@ -7938,10 +7938,10 @@
       <c r="H131" s="3" t="s">
         <v>853</v>
       </c>
-      <c r="I131">
+      <c r="I131" s="4">
         <v>0.79977047443389804</v>
       </c>
-      <c r="J131">
+      <c r="J131" s="4">
         <v>0.86690813302993697</v>
       </c>
       <c r="K131" s="1"/>
@@ -7971,10 +7971,10 @@
       <c r="H132" s="3" t="s">
         <v>608</v>
       </c>
-      <c r="I132">
+      <c r="I132" s="4">
         <v>0.94818335771560602</v>
       </c>
-      <c r="J132">
+      <c r="J132" s="4">
         <v>0.99999997019767695</v>
       </c>
       <c r="K132" s="1"/>
@@ -8004,10 +8004,10 @@
       <c r="H133" s="3" t="s">
         <v>854</v>
       </c>
-      <c r="I133">
+      <c r="I133" s="4">
         <v>0.99778434634208601</v>
       </c>
-      <c r="J133">
+      <c r="J133" s="4">
         <v>0.96642264723777704</v>
       </c>
       <c r="K133" s="1"/>
@@ -8037,10 +8037,10 @@
       <c r="H134" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="I134">
+      <c r="I134" s="4">
         <v>0.92623049020767201</v>
       </c>
-      <c r="J134">
+      <c r="J134" s="4">
         <v>0.92398694157600403</v>
       </c>
       <c r="K134" s="1"/>
@@ -8070,10 +8070,10 @@
       <c r="H135" s="3" t="s">
         <v>855</v>
       </c>
-      <c r="I135">
+      <c r="I135" s="4">
         <v>0.62829440832137995</v>
       </c>
-      <c r="J135">
+      <c r="J135" s="4">
         <v>0.53461752831935805</v>
       </c>
       <c r="K135" s="1"/>
@@ -8103,10 +8103,10 @@
       <c r="H136" s="3" t="s">
         <v>856</v>
       </c>
-      <c r="I136">
+      <c r="I136" s="4">
         <v>0.758783839643001</v>
       </c>
-      <c r="J136">
+      <c r="J136" s="4">
         <v>0.821882784366607</v>
       </c>
       <c r="K136" s="1"/>
@@ -8136,10 +8136,10 @@
       <c r="H137" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="I137">
+      <c r="I137" s="4">
         <v>0.999999940395355</v>
       </c>
-      <c r="J137">
+      <c r="J137" s="4">
         <v>0.999999940395355</v>
       </c>
       <c r="K137" s="1"/>
@@ -8169,10 +8169,10 @@
       <c r="H138" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="I138">
+      <c r="I138" s="4">
         <v>0.94193679094314497</v>
       </c>
-      <c r="J138">
+      <c r="J138" s="4">
         <v>1</v>
       </c>
       <c r="K138" s="1"/>
@@ -8202,10 +8202,10 @@
       <c r="H139" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="I139">
+      <c r="I139" s="4">
         <v>1</v>
       </c>
-      <c r="J139">
+      <c r="J139" s="4">
         <v>0.938443303108215</v>
       </c>
       <c r="K139" s="1"/>
@@ -8235,10 +8235,10 @@
       <c r="H140" s="3" t="s">
         <v>859</v>
       </c>
-      <c r="I140">
+      <c r="I140" s="4">
         <v>0.67404870192209798</v>
       </c>
-      <c r="J140">
+      <c r="J140" s="4">
         <v>0.70402303834756197</v>
       </c>
       <c r="K140" s="1"/>
@@ -8268,10 +8268,10 @@
       <c r="H141" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="I141">
+      <c r="I141" s="4">
         <v>0.85096903642018595</v>
       </c>
-      <c r="J141">
+      <c r="J141" s="4">
         <v>1</v>
       </c>
       <c r="K141" s="1"/>
@@ -8301,10 +8301,10 @@
       <c r="H142" s="3" t="s">
         <v>861</v>
       </c>
-      <c r="I142">
+      <c r="I142" s="4">
         <v>0.82341498136520297</v>
       </c>
-      <c r="J142">
+      <c r="J142" s="4">
         <v>0.89969319105148304</v>
       </c>
       <c r="K142" s="1"/>
@@ -8334,10 +8334,10 @@
       <c r="H143" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="I143">
+      <c r="I143" s="4">
         <v>0.73636556168397205</v>
       </c>
-      <c r="J143">
+      <c r="J143" s="4">
         <v>0.83408801754315698</v>
       </c>
       <c r="K143" s="1"/>
@@ -8367,10 +8367,10 @@
       <c r="H144" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I144">
+      <c r="I144" s="4">
         <v>0.96863827109336798</v>
       </c>
-      <c r="J144">
+      <c r="J144" s="4">
         <v>0.999999940395355</v>
       </c>
       <c r="K144" s="1"/>
@@ -8400,10 +8400,10 @@
       <c r="H145" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I145">
+      <c r="I145" s="4">
         <v>1</v>
       </c>
-      <c r="J145">
+      <c r="J145" s="4">
         <v>1</v>
       </c>
       <c r="K145" s="1"/>
@@ -8433,10 +8433,10 @@
       <c r="H146" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="I146">
+      <c r="I146" s="4">
         <v>1</v>
       </c>
-      <c r="J146">
+      <c r="J146" s="4">
         <v>0.85092353820800704</v>
       </c>
       <c r="K146" s="1"/>
@@ -8466,10 +8466,10 @@
       <c r="H147" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="I147">
+      <c r="I147" s="4">
         <v>0.710384041070938</v>
       </c>
-      <c r="J147">
+      <c r="J147" s="4">
         <v>0.710384041070938</v>
       </c>
       <c r="K147" s="1"/>
@@ -8499,10 +8499,10 @@
       <c r="H148" s="3" t="s">
         <v>863</v>
       </c>
-      <c r="I148">
+      <c r="I148" s="4">
         <v>0.68414294719696001</v>
       </c>
-      <c r="J148">
+      <c r="J148" s="4">
         <v>0.58072590827941895</v>
       </c>
       <c r="K148" s="1"/>
@@ -8532,10 +8532,10 @@
       <c r="H149" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="I149">
+      <c r="I149" s="4">
         <v>0.58628222346305803</v>
       </c>
-      <c r="J149">
+      <c r="J149" s="4">
         <v>0.84739987055460597</v>
       </c>
       <c r="K149" s="1"/>
@@ -8565,10 +8565,10 @@
       <c r="H150" s="3" t="s">
         <v>865</v>
       </c>
-      <c r="I150">
+      <c r="I150" s="4">
         <v>0.9483070174853</v>
       </c>
-      <c r="J150">
+      <c r="J150" s="4">
         <v>0.72003992398579897</v>
       </c>
       <c r="K150" s="1"/>
@@ -8598,10 +8598,10 @@
       <c r="H151" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="I151">
+      <c r="I151" s="4">
         <v>0.72354567050933805</v>
       </c>
-      <c r="J151">
+      <c r="J151" s="4">
         <v>0.82594674825668302</v>
       </c>
       <c r="K151" s="1"/>
@@ -8631,10 +8631,10 @@
       <c r="H152" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="I152">
+      <c r="I152" s="4">
         <v>0.62806189060211104</v>
       </c>
-      <c r="J152">
+      <c r="J152" s="4">
         <v>0.99556875228881803</v>
       </c>
       <c r="K152" s="1"/>
@@ -8664,10 +8664,10 @@
       <c r="H153" s="3" t="s">
         <v>866</v>
       </c>
-      <c r="I153">
+      <c r="I153" s="4">
         <v>0.67971751093864397</v>
       </c>
-      <c r="J153">
+      <c r="J153" s="4">
         <v>0.91852995753288202</v>
       </c>
       <c r="K153" s="1"/>
@@ -8697,10 +8697,10 @@
       <c r="H154" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="I154">
+      <c r="I154" s="4">
         <v>0.56544709205627397</v>
       </c>
-      <c r="J154">
+      <c r="J154" s="4">
         <v>0.99556875228881803</v>
       </c>
       <c r="K154" s="1"/>
@@ -8730,10 +8730,10 @@
       <c r="H155" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="I155">
+      <c r="I155" s="4">
         <v>0.78962790966033902</v>
       </c>
-      <c r="J155">
+      <c r="J155" s="4">
         <v>0.78962790966033902</v>
       </c>
       <c r="K155" s="1"/>
@@ -8763,10 +8763,10 @@
       <c r="H156" s="3" t="s">
         <v>867</v>
       </c>
-      <c r="I156">
+      <c r="I156" s="4">
         <v>0.81780179589986801</v>
       </c>
-      <c r="J156">
+      <c r="J156" s="4">
         <v>0.772245973348617</v>
       </c>
       <c r="K156" s="1"/>
@@ -8796,10 +8796,10 @@
       <c r="H157" s="3" t="s">
         <v>868</v>
       </c>
-      <c r="I157">
+      <c r="I157" s="4">
         <v>0.99063120285669903</v>
       </c>
-      <c r="J157">
+      <c r="J157" s="4">
         <v>0.81967326005299801</v>
       </c>
       <c r="K157" s="1"/>
@@ -8829,10 +8829,10 @@
       <c r="H158" s="3" t="s">
         <v>869</v>
       </c>
-      <c r="I158">
+      <c r="I158" s="4">
         <v>0.68561989068984897</v>
       </c>
-      <c r="J158">
+      <c r="J158" s="4">
         <v>0.68388239542643203</v>
       </c>
       <c r="K158" s="1"/>
@@ -8862,10 +8862,10 @@
       <c r="H159" s="3" t="s">
         <v>870</v>
       </c>
-      <c r="I159">
+      <c r="I159" s="4">
         <v>0.92246052622795105</v>
       </c>
-      <c r="J159">
+      <c r="J159" s="4">
         <v>0.82638618350028903</v>
       </c>
       <c r="K159" s="1"/>
@@ -8895,10 +8895,10 @@
       <c r="H160" s="3" t="s">
         <v>729</v>
       </c>
-      <c r="I160">
+      <c r="I160" s="4">
         <v>0.21724188327789301</v>
       </c>
-      <c r="J160">
+      <c r="J160" s="4">
         <v>0.21724188327789301</v>
       </c>
       <c r="K160" s="1"/>
@@ -8928,10 +8928,10 @@
       <c r="H161" s="3" t="s">
         <v>871</v>
       </c>
-      <c r="I161">
+      <c r="I161" s="4">
         <v>0.54606418311595895</v>
       </c>
-      <c r="J161">
+      <c r="J161" s="4">
         <v>0.821882784366607</v>
       </c>
       <c r="K161" s="1"/>
@@ -8949,10 +8949,10 @@
       <c r="F162" s="4">
         <v>0.22638063132762901</v>
       </c>
-      <c r="I162">
+      <c r="I162" s="4">
         <v>0.22638063132762901</v>
       </c>
-      <c r="J162">
+      <c r="J162" s="4">
         <v>0.22638063132762901</v>
       </c>
       <c r="K162" s="1"/>
@@ -8982,10 +8982,10 @@
       <c r="H163" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="I163">
+      <c r="I163" s="4">
         <v>0.84854403138160694</v>
       </c>
-      <c r="J163">
+      <c r="J163" s="4">
         <v>0.76370081305503801</v>
       </c>
       <c r="K163" s="1"/>
@@ -9015,10 +9015,10 @@
       <c r="H164" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="I164">
+      <c r="I164" s="4">
         <v>0.89224588871002197</v>
       </c>
-      <c r="J164">
+      <c r="J164" s="4">
         <v>0.90734491745630896</v>
       </c>
       <c r="K164" s="1"/>
@@ -9048,10 +9048,10 @@
       <c r="H165" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="I165">
+      <c r="I165" s="4">
         <v>0.37323839962482402</v>
       </c>
-      <c r="J165">
+      <c r="J165" s="4">
         <v>0.35858868807554201</v>
       </c>
       <c r="K165" s="1"/>
@@ -9081,10 +9081,10 @@
       <c r="H166" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="I166">
+      <c r="I166" s="4">
         <v>0.54148606956005096</v>
       </c>
-      <c r="J166">
+      <c r="J166" s="4">
         <v>0.52967828512191695</v>
       </c>
       <c r="K166" s="1"/>
@@ -9114,10 +9114,10 @@
       <c r="H167" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="I167">
+      <c r="I167" s="4">
         <v>1.00000011920928</v>
       </c>
-      <c r="J167">
+      <c r="J167" s="4">
         <v>1.00000011920928</v>
       </c>
       <c r="K167" s="1"/>
@@ -9147,10 +9147,10 @@
       <c r="H168" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="I168">
+      <c r="I168" s="4">
         <v>0.968331158161163</v>
       </c>
-      <c r="J168">
+      <c r="J168" s="4">
         <v>1.00000011920928</v>
       </c>
       <c r="K168" s="1"/>
@@ -9180,10 +9180,10 @@
       <c r="H169" s="3" t="s">
         <v>872</v>
       </c>
-      <c r="I169">
+      <c r="I169" s="4">
         <v>1.00000011920928</v>
       </c>
-      <c r="J169">
+      <c r="J169" s="4">
         <v>0.82742744684219305</v>
       </c>
       <c r="K169" s="1"/>
@@ -9210,10 +9210,10 @@
       <c r="G170" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="I170">
+      <c r="I170" s="4">
         <v>1</v>
       </c>
-      <c r="J170">
+      <c r="J170" s="4">
         <v>0.15849614143371499</v>
       </c>
       <c r="K170" s="1"/>
@@ -9243,10 +9243,10 @@
       <c r="H171" s="3" t="s">
         <v>873</v>
       </c>
-      <c r="I171">
+      <c r="I171" s="4">
         <v>0.89025974273681596</v>
       </c>
-      <c r="J171">
+      <c r="J171" s="4">
         <v>0.78879874944686801</v>
       </c>
       <c r="K171" s="1"/>
@@ -9276,10 +9276,10 @@
       <c r="H172" s="3" t="s">
         <v>874</v>
       </c>
-      <c r="I172">
+      <c r="I172" s="4">
         <v>0.65325050055980605</v>
       </c>
-      <c r="J172">
+      <c r="J172" s="4">
         <v>0.732281774282455</v>
       </c>
       <c r="K172" s="1"/>
@@ -9309,10 +9309,10 @@
       <c r="H173" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="I173">
+      <c r="I173" s="4">
         <v>0.72151819864908795</v>
       </c>
-      <c r="J173">
+      <c r="J173" s="4">
         <v>0.83881005644798201</v>
       </c>
       <c r="K173" s="1"/>
@@ -9342,10 +9342,10 @@
       <c r="H174" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="I174">
+      <c r="I174" s="4">
         <v>0.48693448305129999</v>
       </c>
-      <c r="J174">
+      <c r="J174" s="4">
         <v>0.48693448305129999</v>
       </c>
       <c r="K174" s="1"/>
@@ -9375,10 +9375,10 @@
       <c r="H175" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="I175">
+      <c r="I175" s="4">
         <v>0.80700710415840105</v>
       </c>
-      <c r="J175">
+      <c r="J175" s="4">
         <v>0.94921699166297901</v>
       </c>
       <c r="K175" s="1"/>
@@ -9408,10 +9408,10 @@
       <c r="H176" s="3" t="s">
         <v>875</v>
       </c>
-      <c r="I176">
+      <c r="I176" s="4">
         <v>0.81574066877365103</v>
       </c>
-      <c r="J176">
+      <c r="J176" s="4">
         <v>0.86112469434738104</v>
       </c>
       <c r="K176" s="1"/>
@@ -9441,10 +9441,10 @@
       <c r="H177" s="3" t="s">
         <v>876</v>
       </c>
-      <c r="I177">
+      <c r="I177" s="4">
         <v>0.83469861745834295</v>
       </c>
-      <c r="J177">
+      <c r="J177" s="4">
         <v>0.86524339516957605</v>
       </c>
       <c r="K177" s="1"/>
@@ -9474,10 +9474,10 @@
       <c r="H178" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I178">
+      <c r="I178" s="4">
         <v>0.84506872296333302</v>
       </c>
-      <c r="J178">
+      <c r="J178" s="4">
         <v>0.83757075667381198</v>
       </c>
       <c r="K178" s="1"/>
@@ -9507,10 +9507,10 @@
       <c r="H179" s="3" t="s">
         <v>877</v>
       </c>
-      <c r="I179">
+      <c r="I179" s="4">
         <v>0.95287692546844405</v>
       </c>
-      <c r="J179">
+      <c r="J179" s="4">
         <v>0.66597452759742704</v>
       </c>
       <c r="K179" s="1"/>
@@ -9540,10 +9540,10 @@
       <c r="H180" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I180">
+      <c r="I180" s="4">
         <v>0.84659627079963595</v>
       </c>
-      <c r="J180">
+      <c r="J180" s="4">
         <v>1</v>
       </c>
       <c r="K180" s="1"/>
@@ -9573,10 +9573,10 @@
       <c r="H181" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="I181">
+      <c r="I181" s="4">
         <v>0.42984095215797402</v>
       </c>
-      <c r="J181">
+      <c r="J181" s="4">
         <v>0.74314790964126498</v>
       </c>
       <c r="K181" s="1"/>
@@ -9606,10 +9606,10 @@
       <c r="H182" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="I182">
+      <c r="I182" s="4">
         <v>0.76020756363868702</v>
       </c>
-      <c r="J182">
+      <c r="J182" s="4">
         <v>0.76020756363868702</v>
       </c>
       <c r="K182" s="1"/>
@@ -9639,10 +9639,10 @@
       <c r="H183" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="I183">
+      <c r="I183" s="4">
         <v>0.98436763882637002</v>
       </c>
-      <c r="J183">
+      <c r="J183" s="4">
         <v>0.98381638526916504</v>
       </c>
       <c r="K183" s="1"/>
@@ -9672,10 +9672,10 @@
       <c r="H184" s="3" t="s">
         <v>878</v>
       </c>
-      <c r="I184">
+      <c r="I184" s="4">
         <v>0.77955016493797302</v>
       </c>
-      <c r="J184">
+      <c r="J184" s="4">
         <v>0.27403016388416201</v>
       </c>
       <c r="K184" s="1"/>
@@ -9705,10 +9705,10 @@
       <c r="H185" s="3" t="s">
         <v>879</v>
       </c>
-      <c r="I185">
+      <c r="I185" s="4">
         <v>0.60584956407546997</v>
       </c>
-      <c r="J185">
+      <c r="J185" s="4">
         <v>0.50697100162506104</v>
       </c>
       <c r="K185" s="1"/>
@@ -9738,10 +9738,10 @@
       <c r="H186" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I186">
+      <c r="I186" s="4">
         <v>1</v>
       </c>
-      <c r="J186">
+      <c r="J186" s="4">
         <v>1</v>
       </c>
       <c r="K186" s="1"/>
@@ -9771,10 +9771,10 @@
       <c r="H187" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="I187">
+      <c r="I187" s="4">
         <v>0.81191072861353497</v>
       </c>
-      <c r="J187">
+      <c r="J187" s="4">
         <v>0.65561620394388798</v>
       </c>
       <c r="K187" s="1"/>
@@ -9804,10 +9804,10 @@
       <c r="H188" s="3" t="s">
         <v>880</v>
       </c>
-      <c r="I188">
+      <c r="I188" s="4">
         <v>0.62485489249229398</v>
       </c>
-      <c r="J188">
+      <c r="J188" s="4">
         <v>0.77631458044052104</v>
       </c>
       <c r="K188" s="1"/>
@@ -9837,10 +9837,10 @@
       <c r="H189" s="3" t="s">
         <v>881</v>
       </c>
-      <c r="I189">
+      <c r="I189" s="4">
         <v>0.73123207688331604</v>
       </c>
-      <c r="J189">
+      <c r="J189" s="4">
         <v>0.68117920557657796</v>
       </c>
       <c r="K189" s="1"/>
@@ -9870,10 +9870,10 @@
       <c r="H190" s="3" t="s">
         <v>882</v>
       </c>
-      <c r="I190">
+      <c r="I190" s="4">
         <v>0.76865303516387895</v>
       </c>
-      <c r="J190">
+      <c r="J190" s="4">
         <v>0.82963083187738995</v>
       </c>
       <c r="K190" s="1"/>
@@ -9903,10 +9903,10 @@
       <c r="H191" s="3" t="s">
         <v>883</v>
       </c>
-      <c r="I191">
+      <c r="I191" s="4">
         <v>0.67320561408996504</v>
       </c>
-      <c r="J191">
+      <c r="J191" s="4">
         <v>0.55533318966627099</v>
       </c>
       <c r="K191" s="1"/>
@@ -9936,10 +9936,10 @@
       <c r="H192" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="I192">
+      <c r="I192" s="4">
         <v>0.96040034294128396</v>
       </c>
-      <c r="J192">
+      <c r="J192" s="4">
         <v>0.93727654218673695</v>
       </c>
       <c r="K192" s="1"/>
@@ -9969,10 +9969,10 @@
       <c r="H193" s="3" t="s">
         <v>884</v>
       </c>
-      <c r="I193">
+      <c r="I193" s="4">
         <v>0.70200463136037194</v>
       </c>
-      <c r="J193">
+      <c r="J193" s="4">
         <v>0.69969362020492498</v>
       </c>
       <c r="K193" s="1"/>
@@ -10002,10 +10002,10 @@
       <c r="H194" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="I194">
+      <c r="I194" s="4">
         <v>0.459173634648323</v>
       </c>
-      <c r="J194">
+      <c r="J194" s="4">
         <v>0.66044718027114802</v>
       </c>
       <c r="K194" s="1"/>
@@ -10035,10 +10035,10 @@
       <c r="H195" s="3" t="s">
         <v>885</v>
       </c>
-      <c r="I195">
+      <c r="I195" s="4">
         <v>0.86885114510854</v>
       </c>
-      <c r="J195">
+      <c r="J195" s="4">
         <v>0.77700408299764001</v>
       </c>
       <c r="K195" s="1"/>
@@ -10068,10 +10068,10 @@
       <c r="H196" s="3" t="s">
         <v>886</v>
       </c>
-      <c r="I196">
+      <c r="I196" s="4">
         <v>0.71428243319193496</v>
       </c>
-      <c r="J196">
+      <c r="J196" s="4">
         <v>0.64549316962559999</v>
       </c>
       <c r="K196" s="1"/>
@@ -10101,10 +10101,10 @@
       <c r="H197" s="3" t="s">
         <v>887</v>
       </c>
-      <c r="I197">
+      <c r="I197" s="4">
         <v>0.81755942106246904</v>
       </c>
-      <c r="J197">
+      <c r="J197" s="4">
         <v>0.66743598381678204</v>
       </c>
       <c r="K197" s="1"/>
@@ -10134,10 +10134,10 @@
       <c r="H198" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="I198">
+      <c r="I198" s="4">
         <v>0.96863827109336798</v>
       </c>
-      <c r="J198">
+      <c r="J198" s="4">
         <v>0.96863827109336798</v>
       </c>
       <c r="K198" s="1"/>
@@ -10167,10 +10167,10 @@
       <c r="H199" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I199">
+      <c r="I199" s="4">
         <v>1</v>
       </c>
-      <c r="J199">
+      <c r="J199" s="4">
         <v>1</v>
       </c>
       <c r="K199" s="1"/>
@@ -10200,10 +10200,10 @@
       <c r="H200" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="I200">
+      <c r="I200" s="4">
         <v>0.19616658985614699</v>
       </c>
-      <c r="J200">
+      <c r="J200" s="4">
         <v>0.19616658985614699</v>
       </c>
       <c r="K200" s="1"/>
@@ -10233,10 +10233,10 @@
       <c r="H201" s="3" t="s">
         <v>888</v>
       </c>
-      <c r="I201">
+      <c r="I201" s="4">
         <v>0.313568234443664</v>
       </c>
-      <c r="J201">
+      <c r="J201" s="4">
         <v>0.44867601990699701</v>
       </c>
       <c r="K201" s="1"/>
@@ -10266,10 +10266,10 @@
       <c r="H202" s="3" t="s">
         <v>889</v>
       </c>
-      <c r="I202">
+      <c r="I202" s="4">
         <v>0.84535937756299895</v>
       </c>
-      <c r="J202">
+      <c r="J202" s="4">
         <v>0.79834912220637</v>
       </c>
       <c r="K202" s="1"/>
@@ -10299,10 +10299,10 @@
       <c r="H203" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I203">
+      <c r="I203" s="4">
         <v>0.999999940395355</v>
       </c>
-      <c r="J203">
+      <c r="J203" s="4">
         <v>0.999999940395355</v>
       </c>
       <c r="K203" s="1"/>
@@ -10332,10 +10332,10 @@
       <c r="H204" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="I204">
+      <c r="I204" s="4">
         <v>0.95892767608165697</v>
       </c>
-      <c r="J204">
+      <c r="J204" s="4">
         <v>0.94523686170578003</v>
       </c>
       <c r="K204" s="1"/>
@@ -10365,10 +10365,10 @@
       <c r="H205" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="I205">
+      <c r="I205" s="4">
         <v>0.63155215978622403</v>
       </c>
-      <c r="J205">
+      <c r="J205" s="4">
         <v>0.58313858509063698</v>
       </c>
       <c r="K205" s="1"/>
@@ -10398,10 +10398,10 @@
       <c r="H206" s="3" t="s">
         <v>890</v>
       </c>
-      <c r="I206">
+      <c r="I206" s="4">
         <v>0.82931458950042702</v>
       </c>
-      <c r="J206">
+      <c r="J206" s="4">
         <v>0.89023675521214796</v>
       </c>
       <c r="K206" s="1"/>
@@ -10431,10 +10431,10 @@
       <c r="H207" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="I207">
+      <c r="I207" s="4">
         <v>0.863695949316024</v>
       </c>
-      <c r="J207">
+      <c r="J207" s="4">
         <v>0.94807181755701697</v>
       </c>
       <c r="K207" s="1"/>
@@ -10464,10 +10464,10 @@
       <c r="H208" s="3" t="s">
         <v>892</v>
       </c>
-      <c r="I208">
+      <c r="I208" s="4">
         <v>0.89740037918090798</v>
       </c>
-      <c r="J208">
+      <c r="J208" s="4">
         <v>0.79534319043159396</v>
       </c>
       <c r="K208" s="1"/>
@@ -10497,10 +10497,10 @@
       <c r="H209" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="I209">
+      <c r="I209" s="4">
         <v>0.72499096393585205</v>
       </c>
-      <c r="J209">
+      <c r="J209" s="4">
         <v>0.72499096393585205</v>
       </c>
       <c r="K209" s="1"/>
@@ -10530,10 +10530,10 @@
       <c r="H210" s="3" t="s">
         <v>893</v>
       </c>
-      <c r="I210">
+      <c r="I210" s="4">
         <v>0.83975586295127802</v>
       </c>
-      <c r="J210">
+      <c r="J210" s="4">
         <v>1.00000011920928</v>
       </c>
       <c r="K210" s="1"/>
@@ -10563,10 +10563,10 @@
       <c r="H211" s="3" t="s">
         <v>894</v>
       </c>
-      <c r="I211">
+      <c r="I211" s="4">
         <v>0.83974320888519205</v>
       </c>
-      <c r="J211">
+      <c r="J211" s="4">
         <v>0.68599148839712099</v>
       </c>
       <c r="K211" s="1"/>
@@ -10596,10 +10596,10 @@
       <c r="H212" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="I212">
+      <c r="I212" s="4">
         <v>0.80798524618148804</v>
       </c>
-      <c r="J212">
+      <c r="J212" s="4">
         <v>0.77475973963737399</v>
       </c>
       <c r="K212" s="1"/>
@@ -10629,10 +10629,10 @@
       <c r="H213" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="I213">
+      <c r="I213" s="4">
         <v>0.69925747811794203</v>
       </c>
-      <c r="J213">
+      <c r="J213" s="4">
         <v>0.83881008625030495</v>
       </c>
       <c r="K213" s="1"/>
@@ -10662,10 +10662,10 @@
       <c r="H214" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="I214">
+      <c r="I214" s="4">
         <v>0.67951172590255704</v>
       </c>
-      <c r="J214">
+      <c r="J214" s="4">
         <v>0.74792122840881303</v>
       </c>
       <c r="K214" s="1"/>
@@ -10695,10 +10695,10 @@
       <c r="H215" s="3" t="s">
         <v>895</v>
       </c>
-      <c r="I215">
+      <c r="I215" s="4">
         <v>0.93994542956352201</v>
       </c>
-      <c r="J215">
+      <c r="J215" s="4">
         <v>0.80255869030952398</v>
       </c>
       <c r="K215" s="1"/>
@@ -10728,10 +10728,10 @@
       <c r="H216" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I216">
+      <c r="I216" s="4">
         <v>0.97909222046534194</v>
       </c>
-      <c r="J216">
+      <c r="J216" s="4">
         <v>0.64770975708961398</v>
       </c>
       <c r="K216" s="1"/>
@@ -10761,10 +10761,10 @@
       <c r="H217" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="I217">
+      <c r="I217" s="4">
         <v>0.82175109783808298</v>
       </c>
-      <c r="J217">
+      <c r="J217" s="4">
         <v>0.96863827109336798</v>
       </c>
       <c r="K217" s="1"/>
@@ -10794,10 +10794,10 @@
       <c r="H218" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="I218">
+      <c r="I218" s="4">
         <v>0.70787286758422796</v>
       </c>
-      <c r="J218">
+      <c r="J218" s="4">
         <v>0.84569850564002902</v>
       </c>
       <c r="K218" s="1"/>
@@ -10827,10 +10827,10 @@
       <c r="H219" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="I219">
+      <c r="I219" s="4">
         <v>0.94921708106994596</v>
       </c>
-      <c r="J219">
+      <c r="J219" s="4">
         <v>1.0000000596046399</v>
       </c>
       <c r="K219" s="1"/>
@@ -10860,10 +10860,10 @@
       <c r="H220" s="3" t="s">
         <v>897</v>
       </c>
-      <c r="I220">
+      <c r="I220" s="4">
         <v>0.52100457251071897</v>
       </c>
-      <c r="J220">
+      <c r="J220" s="4">
         <v>0.44375108182430201</v>
       </c>
       <c r="K220" s="1"/>
@@ -10893,10 +10893,10 @@
       <c r="H221" s="3" t="s">
         <v>898</v>
       </c>
-      <c r="I221">
+      <c r="I221" s="4">
         <v>0.99778437614440896</v>
       </c>
-      <c r="J221">
+      <c r="J221" s="4">
         <v>0.99778437614440896</v>
       </c>
       <c r="K221" s="1"/>
@@ -10926,10 +10926,10 @@
       <c r="H222" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="I222">
+      <c r="I222" s="4">
         <v>0.73500726620356205</v>
       </c>
-      <c r="J222">
+      <c r="J222" s="4">
         <v>0.71404698491096497</v>
       </c>
       <c r="K222" s="1"/>
@@ -10956,10 +10956,10 @@
       <c r="H223" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="I223">
+      <c r="I223" s="4">
         <v>0.124797150492668</v>
       </c>
-      <c r="J223">
+      <c r="J223" s="4">
         <v>0.124797150492668</v>
       </c>
       <c r="K223" s="1"/>
@@ -10989,10 +10989,10 @@
       <c r="H224" s="3" t="s">
         <v>899</v>
       </c>
-      <c r="I224">
+      <c r="I224" s="4">
         <v>0.67951172590255704</v>
       </c>
-      <c r="J224">
+      <c r="J224" s="4">
         <v>0.95052355527877797</v>
       </c>
       <c r="K224" s="1"/>
@@ -11022,10 +11022,10 @@
       <c r="H225" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="I225">
+      <c r="I225" s="4">
         <v>0.99778437614440896</v>
       </c>
-      <c r="J225">
+      <c r="J225" s="4">
         <v>0.99778437614440896</v>
       </c>
       <c r="K225" s="1"/>
@@ -11055,10 +11055,10 @@
       <c r="H226" s="3" t="s">
         <v>900</v>
       </c>
-      <c r="I226">
+      <c r="I226" s="4">
         <v>0.89212373892466201</v>
       </c>
-      <c r="J226">
+      <c r="J226" s="4">
         <v>0.86185638606548298</v>
       </c>
       <c r="K226" s="1"/>
@@ -11088,10 +11088,10 @@
       <c r="H227" s="3" t="s">
         <v>901</v>
       </c>
-      <c r="I227">
+      <c r="I227" s="4">
         <v>0.968331158161163</v>
       </c>
-      <c r="J227">
+      <c r="J227" s="4">
         <v>1.00000011920928</v>
       </c>
       <c r="K227" s="1"/>
@@ -11121,10 +11121,10 @@
       <c r="H228" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="I228">
+      <c r="I228" s="4">
         <v>1.0000000298023199</v>
       </c>
-      <c r="J228">
+      <c r="J228" s="4">
         <v>0.78340962529182401</v>
       </c>
       <c r="K228" s="1"/>
@@ -11154,10 +11154,10 @@
       <c r="H229" s="3" t="s">
         <v>902</v>
       </c>
-      <c r="I229">
+      <c r="I229" s="4">
         <v>0.59773597121238697</v>
       </c>
-      <c r="J229">
+      <c r="J229" s="4">
         <v>0.71769918998082405</v>
       </c>
       <c r="K229" s="1"/>
@@ -11187,10 +11187,10 @@
       <c r="H230" s="3" t="s">
         <v>903</v>
       </c>
-      <c r="I230">
+      <c r="I230" s="4">
         <v>0.824435055255889</v>
       </c>
-      <c r="J230">
+      <c r="J230" s="4">
         <v>0.49498690664768202</v>
       </c>
       <c r="K230" s="1"/>
@@ -11220,10 +11220,10 @@
       <c r="H231" s="3" t="s">
         <v>904</v>
       </c>
-      <c r="I231">
+      <c r="I231" s="4">
         <v>0.92246064543724005</v>
       </c>
-      <c r="J231">
+      <c r="J231" s="4">
         <v>0.423325054347515</v>
       </c>
       <c r="K231" s="1"/>
@@ -11253,10 +11253,10 @@
       <c r="H232" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="I232">
+      <c r="I232" s="4">
         <v>0.83344759543736702</v>
       </c>
-      <c r="J232">
+      <c r="J232" s="4">
         <v>0.97909216086069695</v>
       </c>
       <c r="K232" s="1"/>
@@ -11286,10 +11286,10 @@
       <c r="H233" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I233">
+      <c r="I233" s="4">
         <v>0.67762017250061002</v>
       </c>
-      <c r="J233">
+      <c r="J233" s="4">
         <v>0.67762017250061002</v>
       </c>
       <c r="K233" s="1"/>
@@ -11319,10 +11319,10 @@
       <c r="H234" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="I234">
+      <c r="I234" s="4">
         <v>0.53621900081634499</v>
       </c>
-      <c r="J234">
+      <c r="J234" s="4">
         <v>0.53621900081634499</v>
       </c>
       <c r="K234" s="1"/>
@@ -11352,10 +11352,10 @@
       <c r="H235" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I235">
+      <c r="I235" s="4">
         <v>1</v>
       </c>
-      <c r="J235">
+      <c r="J235" s="4">
         <v>1</v>
       </c>
       <c r="K235" s="1"/>
@@ -11385,10 +11385,10 @@
       <c r="H236" s="3" t="s">
         <v>905</v>
       </c>
-      <c r="I236">
+      <c r="I236" s="4">
         <v>0.85806031525134996</v>
       </c>
-      <c r="J236">
+      <c r="J236" s="4">
         <v>0.76608396321535099</v>
       </c>
       <c r="K236" s="1"/>
@@ -11415,10 +11415,10 @@
       <c r="H237" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="I237">
+      <c r="I237" s="4">
         <v>0.67951172590255704</v>
       </c>
-      <c r="J237">
+      <c r="J237" s="4">
         <v>1.00000023841857</v>
       </c>
       <c r="K237" s="1"/>

</xml_diff>